<commit_message>
Update study data results and notebook
</commit_message>
<xml_diff>
--- a/lab/analysis/meditation-study-responses.xlsx
+++ b/lab/analysis/meditation-study-responses.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
   <si>
     <t>Timestamp</t>
   </si>
@@ -132,6 +132,16 @@
     <t>I'm very stressed about school (stressed).</t>
   </si>
   <si>
+    <t>I like Blue/Yellow, it reminds me of a calm sunny day at the beach (yellow is the sun/sand, blue is like a clear ocean in Hawaii) 
+I would try mindful observation, effect-centered or mantra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For the video-audio, I think the movements were quite effective. Personally, I found my eyebrows moving along to the visual movements (which helped relaxed them). 
+I put a 3, for “if music added to experience” because I kind of thought the music was a little bit of a distraction to the person speaking. However, I do like the idea of adding music. 
+I think this somewhat helped with my school stress and anxiety so thank you
+</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
@@ -145,6 +155,33 @@
   </si>
   <si>
     <t>1-3</t>
+  </si>
+  <si>
+    <t>I would add a purple one because it’s a my favorite color and it makes me generally calm. I feel like personalization is important because someone may see red as their favorite while another may see it as anger.</t>
+  </si>
+  <si>
+    <t>The blue yellow one seems relaxing the most!</t>
+  </si>
+  <si>
+    <t>I prefer the yellow/blue one just because the colors are not contrasting = easier on the eyes</t>
+  </si>
+  <si>
+    <t>have a color scheme could make the video more relaxing</t>
+  </si>
+  <si>
+    <t>red orange is nice i would try that</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>10+ and I used to meditate regularly</t>
+  </si>
+  <si>
+    <t>Audio-Video felt higher quality because if felt like more effort was put in</t>
+  </si>
+  <si>
+    <t>Maybe something like red and orange to be easier on the eyes and more relaxing</t>
   </si>
 </sst>
 </file>
@@ -154,7 +191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -165,6 +202,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -181,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -194,6 +235,18 @@
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -620,16 +673,22 @@
       <c r="X3" s="3">
         <v>5.0</v>
       </c>
+      <c r="Y3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
         <v>45210.879685486114</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>26</v>
@@ -638,7 +697,7 @@
         <v>27</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>29</v>
@@ -682,19 +741,20 @@
       <c r="X4" s="3">
         <v>1.0</v>
       </c>
+      <c r="Y4" s="3"/>
     </row>
     <row r="5">
       <c r="A5" s="2">
         <v>45210.887019629634</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D5" s="3">
         <v>0.0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>30</v>
@@ -753,7 +813,7 @@
         <v>24</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>26</v>
@@ -812,13 +872,13 @@
         <v>45212.88697545139</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="3">
         <v>0.0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>30</v>
@@ -867,6 +927,9 @@
       </c>
       <c r="X7" s="3">
         <v>4.0</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8">
@@ -877,10 +940,10 @@
         <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>30</v>
@@ -939,10 +1002,10 @@
         <v>24</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>30</v>
@@ -991,6 +1054,9 @@
       </c>
       <c r="X9" s="3">
         <v>3.0</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10">
@@ -998,13 +1064,13 @@
         <v>45213.16520314815</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" s="3">
         <v>0.0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>30</v>
@@ -1054,6 +1120,370 @@
       <c r="X10" s="3">
         <v>2.0</v>
       </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <v>45214.487230451385</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="M11" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="N11" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="O11" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="P11" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="R11" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="S11" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="T11" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="U11" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="V11" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="W11" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="X11" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <v>45221.08479076389</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="M12" s="8">
+        <v>9.0</v>
+      </c>
+      <c r="N12" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="O12" s="8">
+        <v>9.0</v>
+      </c>
+      <c r="P12" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="R12" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="S12" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="T12" s="8">
+        <v>9.0</v>
+      </c>
+      <c r="U12" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="V12" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="W12" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="X12" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="Y12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <v>45221.10584605324</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="N13" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="O13" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="P13" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="R13" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="S13" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="T13" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="U13" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="V13" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="W13" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="X13" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <v>45223.3865444213</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="M14" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="N14" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="O14" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="P14" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="R14" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="S14" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="T14" s="3">
+        <v>7.0</v>
+      </c>
+      <c r="U14" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="V14" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="W14" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="X14" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <v>45224.609894293986</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="M15" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="N15" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="O15" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="P15" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="R15" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="S15" s="8">
+        <v>7.0</v>
+      </c>
+      <c r="T15" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="U15" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="V15" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="W15" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="X15" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="Y15" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="7"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>